<commit_message>
Fixing minor bug with timestamp on JUNC folders
</commit_message>
<xml_diff>
--- a/OUTPUT.xlsx
+++ b/OUTPUT.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1110</v>
+        <v>1125</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.66036036036036</v>
+        <v>1.347555555555556</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1903</v>
+        <v>1598</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>418</v>
+        <v>193</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>177</v>
+        <v>418</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>498</v>
+        <v>177</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>750</v>
+        <v>728</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -663,11 +663,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DEtl</t>
+          <t>EEr</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>418</v>
+        <v>82</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -681,11 +681,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DEr</t>
+          <t>DStl</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -699,11 +699,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DEl</t>
+          <t>DSt</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -717,11 +717,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CWtl</t>
+          <t>DSrt</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -735,11 +735,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CWrt</t>
+          <t>DSr</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -753,11 +753,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CWr</t>
+          <t>DSl</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -771,11 +771,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CWl</t>
+          <t>CEtl</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>99</v>
+        <v>418</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -789,11 +789,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BStl</t>
+          <t>CEr</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>497</v>
+        <v>418</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -807,11 +807,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BSt</t>
+          <t>CEl</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>498</v>
+        <v>180</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -825,11 +825,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BSrt</t>
+          <t>BWtl</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -843,11 +843,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BSr</t>
+          <t>BWrt</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>9</v>
+        <v>138</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -861,11 +861,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BSl</t>
+          <t>BWr</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -879,11 +879,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ANrt</t>
+          <t>BWl</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>750</v>
+        <v>99</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -897,11 +897,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ANr</t>
+          <t>ANrt</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>107</v>
+        <v>728</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -913,6 +913,14 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ANr</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>107</v>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Recreating the main files
</commit_message>
<xml_diff>
--- a/OUTPUT.xlsx
+++ b/OUTPUT.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1125</v>
+        <v>1800</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1110</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="3">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.347555555555556</v>
+        <v>1.097241379310345</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.36036036036036</v>
+        <v>1.282068965517241</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1598</v>
+        <v>1591</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1746</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="5">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>287</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>418</v>
+        <v>594</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>186</v>
+        <v>615</v>
       </c>
     </row>
     <row r="10">
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>438</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11">
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>728</v>
+        <v>921</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -621,306 +621,166 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>599</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ENrt</t>
+          <t>CSt</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>82</v>
+        <v>594</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>EEtl</t>
+          <t>CNt</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>236</v>
+        <v>615</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ENl</t>
+          <t>CNt</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60</v>
+        <v>594</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>EEr</t>
+          <t>CNl</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>113</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>EEr</t>
+          <t>BEr</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>EEl</t>
+          <t>CEr</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>134</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DStl</t>
+          <t>BEl</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>191</v>
+        <v>76</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>DWtl</t>
+          <t>BEl</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>167</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DSt</t>
+          <t>ANt</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>192</v>
+        <v>921</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>DWrt</t>
+          <t>ASt</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>167</v>
+        <v>774</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DSrt</t>
+          <t>ANl</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>50</v>
+        <v>560</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DWr</t>
+          <t>ANt</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>287</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DSr</t>
+          <t>AEr</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>DWl</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>242</v>
-      </c>
+        <v>609</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>DSl</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>193</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>CNrt</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>186</v>
-      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>CEtl</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>418</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CNr</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>59</v>
-      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CEr</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>418</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>CNl</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>186</v>
-      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CEl</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>180</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>BStl</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>437</v>
-      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>BWtl</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>139</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>BSt</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>438</v>
-      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>BWrt</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>138</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>BSrt</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>50</v>
-      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>BWr</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>177</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>BSr</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>9</v>
-      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>BWl</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>99</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>BSl</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>160</v>
-      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>ANrt</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>728</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>ANrt</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>599</v>
-      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>ANr</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>107</v>
-      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
     </row>

</xml_diff>